<commit_message>
Vanilla Backstories Expanded 수정
#741
한국어 환경에 대응하지 않는 원문 매개변수 수정
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Backstories Expanded - 2861806869/2861806869.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Backstories Expanded - 2861806869/2861806869.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.1\Vanilla Backstories Expanded - 2861806869\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Backstories Expanded - 2861806869\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508D2119-2831-460A-ACCF-57278A9D85EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4934BBF2-4A3B-4D6C-8EE0-59A1D513EEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240429" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240429" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +32,244 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>RimWorldKorea</author>
+  </authors>
+  <commentList>
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{808D4677-CF85-4E6C-93CE-F7D6BD114BEE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>주의</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">]
+PAWN_pronounCap </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>있으면</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>쓰지</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>말거나</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> PAWN_pronoun</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>으로</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>대체하세요</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>한국어</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>환경에선</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>오류를</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>유발합니다</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="1929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="1933">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -5806,9 +6042,6 @@
     <t>[PAWN_nameDef](이)가 옛날부터 부족에 소속되어있지는 않았습니다. [PAWN_possessive] 이방인 조합에서 농사를 담당하다가 농작물 수확을 망친 후, [PAWN_nameDef](은)는 [PAWN_objective] 도울 조잡한 도구만 가지고 몇 년 동안 야외에서 홀로 살아야 했습니다. 이건 [PAWN_objective] 생존에 관해서는 만능인으로 만들었지만, [PAWN_possessive] 사람에 대한 믿음은 완전히 없어졌습니다.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>[PAWN_nameDef](은)는 부드러움과 수면 품질을 제공하는지를 다양한 매트리스에서 평가합니다. 그로 인해 낮잠은 강제적이었습니다.  "세계 최고의 직업".</t>
   </si>
   <si>
@@ -5828,13 +6061,28 @@
   </si>
   <si>
     <t>[PAWN_nameDef](이)가 오랫동안 있던 곳이라면 [PAWN_pronoun] 항상 불행이 따랐습니다. 자연 재해, 습격, 침입, 폭격, 노예화는 자신과 관련된 사람들이 겪어야 했던 일부 사건일 뿐입니다. 그러나 죽음과 파괴를 통해 [PAWN_pronoun] [PAWN_possessive] 내면의 껍질을 뚫고 나아갔습니다.</t>
+  </si>
+  <si>
+    <t>After years of military service, [PAWN_nameDef] retired to the colony seeking peace. Despite [PAWN_possessive] efforts to integrate, [PAWN_pronoun] struggled with non-violent tasks, finding solace only in routine and physical labor. [PAWN_pronoun]'s experience made [PAWN_pronoun] a valuable asset during conflicts, but [PAWN_pronoun] never quite adapted to civilian life.</t>
+  </si>
+  <si>
+    <t>[PAWN_nameDef] oversaw a large botanical garden, specializing in the cultivation of rare plants and educating the public. [PAWN_pronoun]'s green thumb was unparalleled, yet [PAWN_pronoun] lacked the physical capabilities for demanding labor or combat.</t>
+  </si>
+  <si>
+    <t>[PAWN_nameDef] charted the stars as the primary navigator aboard a spacefaring vessel. [PAWN_pronoun] had an uncanny ability to find the safest and quickest routes through the cosmos, though [PAWN_pronoun] struggled with mechanical tasks and often left those to others.</t>
+  </si>
+  <si>
+    <t>[PAWN_nameDef] served as the medic on a spaceship, treating everything from space sickness to injuries from asteroid impacts. [PAWN_pronoun]'s knowledge of medicine was unparalleled, but [PAWN_pronoun] had no head for research or complex theories.</t>
+  </si>
+  <si>
+    <t>[PAWN_nameDef] was responsible for managing the cargo bay of a space vessel, ensuring supplies were securely stowed and inventory was accurately tracked. [PAWN_pronoun] was physically strong and highly organized, but [PAWN_pronoun] had little patience for detailed documentation or scholarly pursuits.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5853,16 +6101,55 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -5870,15 +6157,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="메모" xfId="2" builtinId="10"/>
+    <cellStyle name="보통" xfId="1" builtinId="28"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6178,11 +6490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F523"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4376F6A1-69C9-463A-BDA2-6CCC1AB6FB1F}">
+  <dimension ref="A1:G523"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -6191,12 +6503,12 @@
     <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="108.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="40.6328125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6216,7 +6528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -6229,11 +6541,8 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -6246,11 +6555,8 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -6263,11 +6569,8 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -6280,11 +6583,8 @@
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -6297,11 +6597,8 @@
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -6314,11 +6611,12 @@
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F7" s="2" t="s">
+        <v>1928</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -6331,11 +6629,8 @@
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -6348,11 +6643,8 @@
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -6365,11 +6657,8 @@
       <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -6382,11 +6671,8 @@
       <c r="E11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -6399,11 +6685,8 @@
       <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -6416,11 +6699,11 @@
       <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F13" s="2" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -6433,11 +6716,8 @@
       <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -6450,11 +6730,8 @@
       <c r="E15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -6466,9 +6743,6 @@
       </c>
       <c r="E16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1921</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -6484,9 +6758,6 @@
       <c r="E17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
@@ -6501,9 +6772,6 @@
       <c r="E18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
@@ -6518,8 +6786,8 @@
       <c r="E19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>1921</v>
+      <c r="F19" s="2" t="s">
+        <v>1930</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -6535,9 +6803,6 @@
       <c r="E20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
@@ -6552,9 +6817,6 @@
       <c r="E21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
@@ -6569,9 +6831,6 @@
       <c r="E22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
@@ -6586,9 +6845,6 @@
       <c r="E23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
@@ -6603,9 +6859,6 @@
       <c r="E24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
@@ -6620,8 +6873,8 @@
       <c r="E25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>1921</v>
+      <c r="F25" s="2" t="s">
+        <v>1931</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -6637,9 +6890,6 @@
       <c r="E26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
@@ -6654,9 +6904,6 @@
       <c r="E27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
@@ -6671,8 +6918,8 @@
       <c r="E28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>1921</v>
+      <c r="F28" s="2" t="s">
+        <v>1932</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -6688,9 +6935,6 @@
       <c r="E29" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
@@ -6705,9 +6949,6 @@
       <c r="E30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
@@ -6722,9 +6963,6 @@
       <c r="E31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>1921</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
@@ -6739,11 +6977,8 @@
       <c r="E32" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
@@ -6756,11 +6991,8 @@
       <c r="E33" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>102</v>
       </c>
@@ -6773,11 +7005,8 @@
       <c r="E34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>105</v>
       </c>
@@ -6790,11 +7019,8 @@
       <c r="E35" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>108</v>
       </c>
@@ -6807,11 +7033,8 @@
       <c r="E36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>111</v>
       </c>
@@ -6824,11 +7047,8 @@
       <c r="E37" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>114</v>
       </c>
@@ -6841,11 +7061,8 @@
       <c r="E38" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>117</v>
       </c>
@@ -6858,11 +7075,8 @@
       <c r="E39" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>120</v>
       </c>
@@ -6875,11 +7089,8 @@
       <c r="E40" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>123</v>
       </c>
@@ -6892,11 +7103,8 @@
       <c r="E41" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>126</v>
       </c>
@@ -6909,11 +7117,8 @@
       <c r="E42" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>129</v>
       </c>
@@ -6926,11 +7131,8 @@
       <c r="E43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>132</v>
       </c>
@@ -6943,11 +7145,8 @@
       <c r="E44" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>135</v>
       </c>
@@ -6960,11 +7159,8 @@
       <c r="E45" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>138</v>
       </c>
@@ -6977,11 +7173,8 @@
       <c r="E46" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
@@ -6994,11 +7187,8 @@
       <c r="E47" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -7011,11 +7201,8 @@
       <c r="E48" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -7028,11 +7215,8 @@
       <c r="E49" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -7045,11 +7229,8 @@
       <c r="E50" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
@@ -7062,11 +7243,8 @@
       <c r="E51" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>156</v>
       </c>
@@ -7079,11 +7257,8 @@
       <c r="E52" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>159</v>
       </c>
@@ -7096,11 +7271,8 @@
       <c r="E53" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>162</v>
       </c>
@@ -7113,11 +7285,8 @@
       <c r="E54" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>165</v>
       </c>
@@ -7130,11 +7299,8 @@
       <c r="E55" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>168</v>
       </c>
@@ -7147,11 +7313,8 @@
       <c r="E56" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>171</v>
       </c>
@@ -7164,11 +7327,8 @@
       <c r="E57" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>174</v>
       </c>
@@ -7181,11 +7341,8 @@
       <c r="E58" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>177</v>
       </c>
@@ -7198,11 +7355,8 @@
       <c r="E59" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>180</v>
       </c>
@@ -7215,11 +7369,8 @@
       <c r="E60" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>183</v>
       </c>
@@ -7232,11 +7383,8 @@
       <c r="E61" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>186</v>
       </c>
@@ -7249,11 +7397,8 @@
       <c r="E62" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>189</v>
       </c>
@@ -7266,11 +7411,8 @@
       <c r="E63" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>191</v>
       </c>
@@ -7282,9 +7424,6 @@
       </c>
       <c r="E64" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>1921</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -9222,7 +9361,7 @@
         <v>527</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.45">
@@ -9681,7 +9820,7 @@
         <v>605</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.45">
@@ -9936,7 +10075,7 @@
         <v>648</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.45">
@@ -11721,7 +11860,7 @@
         <v>950</v>
       </c>
       <c r="F325" s="1" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="326" spans="1:6" x14ac:dyDescent="0.45">
@@ -12129,7 +12268,7 @@
         <v>1020</v>
       </c>
       <c r="F349" s="1" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="350" spans="1:6" x14ac:dyDescent="0.45">
@@ -12180,7 +12319,7 @@
         <v>1029</v>
       </c>
       <c r="F352" s="1" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="353" spans="1:6" x14ac:dyDescent="0.45">
@@ -13965,7 +14104,7 @@
         <v>1333</v>
       </c>
       <c r="F457" s="1" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.45">
@@ -15093,5 +15232,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>